<commit_message>
Fixing Read Excel, Add page helper
</commit_message>
<xml_diff>
--- a/Resources/QuickAcq Testplan.xlsx
+++ b/Resources/QuickAcq Testplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Data\Project\selenium\dotnet\LatihanSelenium\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B51303-334E-4DF6-AF69-955E0D2A02F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B232FF17-48D3-49F8-8336-1E3E098B3F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="2160" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>Module Name</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>Action</t>
-  </si>
-  <si>
-    <t>Return To</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>Result</t>
@@ -673,10 +667,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -684,7 +678,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -696,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -704,7 +698,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -716,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -725,16 +719,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -742,64 +736,64 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -846,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -925,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -937,7 +931,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -945,7 +939,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -995,7 +989,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1008,13 +1002,12 @@
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="56.28515625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1027,20 +1020,17 @@
       <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1048,16 +1038,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1065,12 +1055,12 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1136,55 +1126,55 @@
         <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1195,25 +1185,25 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K2" s="3">
         <v>1</v>
@@ -1222,7 +1212,7 @@
         <v>20000</v>
       </c>
       <c r="M2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -1231,7 +1221,7 @@
         <v>30000</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1242,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -1251,7 +1241,7 @@
         <v>2400</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -1260,7 +1250,7 @@
         <v>3400000</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1271,7 +1261,7 @@
         <v>11</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -1280,7 +1270,7 @@
         <v>45000</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1288,7 +1278,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1299,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1310,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1321,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Add handler confirmation alert
</commit_message>
<xml_diff>
--- a/Resources/QuickAcq Testplan.xlsx
+++ b/Resources/QuickAcq Testplan.xlsx
@@ -3,8 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Data\Project\selenium\dotnet\LatihanSelenium\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE98A1BB-8F98-4A35-ABD0-9DBD17AB11A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="9" r:id="rId1"/>
@@ -14,16 +20,16 @@
     <sheet name="PurchaseRequest" sheetId="19" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1"><![CDATA[TestPlan!$A$1:$K$2]]></definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestPlan!$A$1:$K$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr autoRecover="0" crashSave="0" dataExtractLoad="0" repairLoad="0"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -38,246 +44,246 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
-  <si>
-    <t xml:space="preserve">Module Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From Test Case Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screen Capture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screenshot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data For</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attachment Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P@ssw0rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request For Quotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor Quotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save As Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalog / Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Catalog / Non-Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct Purchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Pending Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discard Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Re Submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods VAT Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services VAT Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pensil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penghapus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License Windows 11 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License Windows 10 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resubmit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\match\Downloads\GRUx6dEbcAAcC6A.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR/2025/01/0005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approve 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approve 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Test Case Id</t>
+  </si>
+  <si>
+    <t>From Test Case Id</t>
+  </si>
+  <si>
+    <t>Date Test</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Screen Capture</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Data For</t>
+  </si>
+  <si>
+    <t>Attachment Path</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Aris</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Purchase Request</t>
+  </si>
+  <si>
+    <t>Request For Quotation</t>
+  </si>
+  <si>
+    <t>Vendor Quotation</t>
+  </si>
+  <si>
+    <t>Vendor Selection</t>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>ROGS</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Save As Draft</t>
+  </si>
+  <si>
+    <t>Submit Draft</t>
+  </si>
+  <si>
+    <t>PR Type</t>
+  </si>
+  <si>
+    <t>Catalog / Contract</t>
+  </si>
+  <si>
+    <t>Non-Catalog / Non-Contract</t>
+  </si>
+  <si>
+    <t>Direct Purchase</t>
+  </si>
+  <si>
+    <t>Search List</t>
+  </si>
+  <si>
+    <t>Search Pending Task</t>
+  </si>
+  <si>
+    <t>Update Draft</t>
+  </si>
+  <si>
+    <t>Discard Draft</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Re Submit</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>PR Subject</t>
+  </si>
+  <si>
+    <t>Required Date</t>
+  </si>
+  <si>
+    <t>Project Code</t>
+  </si>
+  <si>
+    <t>Goods Item Name</t>
+  </si>
+  <si>
+    <t>Goods Item Qty</t>
+  </si>
+  <si>
+    <t>Goods Item Price</t>
+  </si>
+  <si>
+    <t>Services Item Name</t>
+  </si>
+  <si>
+    <t>Services Item Qty</t>
+  </si>
+  <si>
+    <t>Services Item Price</t>
+  </si>
+  <si>
+    <t>Goods VAT Rate</t>
+  </si>
+  <si>
+    <t>Services VAT Rate</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>12 Jan 2025</t>
+  </si>
+  <si>
+    <t>PC22</t>
+  </si>
+  <si>
+    <t>Pensil</t>
+  </si>
+  <si>
+    <t>Buku</t>
+  </si>
+  <si>
+    <t>Penghapus</t>
+  </si>
+  <si>
+    <t>License Windows 11 Pro</t>
+  </si>
+  <si>
+    <t>License Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Resubmit</t>
+  </si>
+  <si>
+    <t>C:\Users\match\Downloads\GRUx6dEbcAAcC6A.jpg</t>
+  </si>
+  <si>
+    <t>PR/2025/01/0005</t>
+  </si>
+  <si>
+    <t>Document Number</t>
+  </si>
+  <si>
+    <t>Approve 1</t>
+  </si>
+  <si>
+    <t>Approve 2</t>
   </si>
   <si>
     <t xml:space="preserve">Reject </t>
@@ -286,7 +292,7 @@
     <t xml:space="preserve">Success approve </t>
   </si>
   <si>
-    <t xml:space="preserve">Task Approve Purchase Request is Fail. Error : Search Task Purchase Request failed: OpenQA.Selenium.WebDriverTimeoutException: Timed out after 60 seconds
+    <t>Task Approve Purchase Request is Fail. Error : Search Task Purchase Request failed: OpenQA.Selenium.WebDriverTimeoutException: Timed out after 60 seconds
  ---&gt; OpenQA.Selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@class='wrapper-pr-pending-task-list']//input[@placeholder='Search']"}
   (Session info: chrome=131.0.6778.265); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
    at OpenQA.Selenium.WebDriver.UnpackAndThrowOnError(Response errorResponse, String commandToExecute)
@@ -301,57 +307,62 @@
    at LatihanSelenium.Utilities.AutomationHelpers.ElementExist(IWebDriver driver, By locator, Int32 sec) in D:\AutomatedTestingQuickAcq\LatihanSelenium\Utilities\AutomationHelpers.cs:line 134</t>
   </si>
   <si>
-    <t xml:space="preserve">Open File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025/01/20 10:36:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approval Purchase Request is Fail. Error : One or more sequences have failed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go To Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Approve Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR/TEST/20/1/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT - Information Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test2012025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard Pulpen AE-7 (Pulpen) Alfa Tip Black 0.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\Kenny Nathaniel\Downloads\lockscreentemp.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025/01/20 12:04:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task Approve Purchase Request is Fail. Error : Notes parameter cannot be empty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025/01/20 13:28:21</t>
+    <t>Open File</t>
+  </si>
+  <si>
+    <t>2025/01/20 10:36:53</t>
+  </si>
+  <si>
+    <t>Approval Purchase Request is Fail. Error : One or more sequences have failed.</t>
+  </si>
+  <si>
+    <t>Go To Data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Approve Test</t>
+  </si>
+  <si>
+    <t>PR/TEST/20/1/2025</t>
+  </si>
+  <si>
+    <t>IT - Information Technology</t>
+  </si>
+  <si>
+    <t>Test2012025</t>
+  </si>
+  <si>
+    <t>Testing Remarks</t>
+  </si>
+  <si>
+    <t>Standard Pulpen AE-7 (Pulpen) Alfa Tip Black 0.5mm</t>
+  </si>
+  <si>
+    <t>C:\Users\Kenny Nathaniel\Downloads\lockscreentemp.jpg</t>
+  </si>
+  <si>
+    <t>2025/01/20 12:04:07</t>
+  </si>
+  <si>
+    <t>Approve test 1</t>
+  </si>
+  <si>
+    <t>Success - Approve with Document Number : PR/2025/01/0005</t>
+  </si>
+  <si>
+    <t>2025/01/20 13:48:54</t>
+  </si>
+  <si>
+    <t>Approval Purchase Request is Successfully.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +389,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -396,10 +415,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,18 +456,22 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -715,8 +739,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -882,8 +906,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -911,16 +935,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -931,12 +955,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,14 +1017,14 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="10">
@@ -1019,140 +1043,142 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2"/>
+  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="0" count="1">
-    <dataValidation type="list" errorStyle="stop" imeMode="noControl" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1><![CDATA[$A$2:$A$1048576]]></formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>$A$2:$A$1048576</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="I3" location="Task!A3" display="Go To Data"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="I4" location="Task!A6" display="Go To Data"/>
-    <hyperlink ref="H5" r:id="rId3"/>
-    <hyperlink ref="I5" location="Task!A7"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" location="Task!A3" display="Go To Data" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I4" location="Task!A6" display="Go To Data" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I5" location="Task!A7" display="Go To Data" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="I5" location="Task!A7" display="Go To Data" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="4">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DFF4BBE4-322C-43AA-907B-7E8804C69D29}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DFF4BBE4-322C-43AA-907B-7E8804C69D29}">
           <x14:formula1>
             <xm:f>Config!$A$2:$A$1000</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE1FC543-0F99-4865-B769-7910654B9523}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE1FC543-0F99-4865-B769-7910654B9523}">
           <x14:formula1>
             <xm:f>Config!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0065DB-CFB7-4F2F-8F2C-0BC39A6E984A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0065DB-CFB7-4F2F-8F2C-0BC39A6E984A}">
           <x14:formula1>
             <xm:f>User!$B$2:$B$50</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8352D6F0-1E94-47AA-9154-FEE416D3592C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8352D6F0-1E94-47AA-9154-FEE416D3592C}">
           <x14:formula1>
             <xm:f>Config!$B$2:$B$20</xm:f>
           </x14:formula1>
@@ -1165,13 +1191,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,19 +1234,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -1228,134 +1254,137 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="E7" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
-    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="4">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
           <x14:formula1>
             <xm:f>User!$B$2:$B$100</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000004000000}">
           <x14:formula1>
             <xm:f>TestPlan!$A$2:$A$99538</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3E39EE4-6441-4C23-BDD7-10E1293E5F03}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3E39EE4-6441-4C23-BDD7-10E1293E5F03}">
           <x14:formula1>
             <xm:f>Config!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCAF1936-EB14-4904-9946-DB0E2AD5F326}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCAF1936-EB14-4904-9946-DB0E2AD5F326}">
           <x14:formula1>
             <xm:f>Config!$F$2:$F$29</xm:f>
           </x14:formula1>
@@ -1368,8 +1397,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:S9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1479,13 +1508,13 @@
       <c r="L2" s="3">
         <v>20000</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="0">
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="O2" s="0">
+      <c r="O2">
         <v>30000</v>
       </c>
       <c r="R2" s="6" t="s">
@@ -1508,13 +1537,13 @@
       <c r="L3" s="3">
         <v>2400</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="0">
+      <c r="N3">
         <v>2</v>
       </c>
-      <c r="O3" s="0">
+      <c r="O3">
         <v>3400000</v>
       </c>
       <c r="R3" s="6" t="s">
@@ -1616,16 +1645,16 @@
       <c r="K9" s="3">
         <v>1</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" t="s">
         <v>73</v>
       </c>
-      <c r="N9" s="0">
+      <c r="N9">
         <v>2</v>
       </c>
-      <c r="P9" s="0">
+      <c r="P9">
         <v>12</v>
       </c>
-      <c r="Q9" s="0">
+      <c r="Q9">
         <v>12</v>
       </c>
       <c r="R9" s="6" t="s">
@@ -1637,21 +1666,21 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="3">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
             <xm:f>TestPlan!$A$2:$A$99538</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7071961E-2CD6-4886-8EA4-4BE8922E8D26}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7071961E-2CD6-4886-8EA4-4BE8922E8D26}">
           <x14:formula1>
             <xm:f>Config!$D$2:$D$999</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9023320-1073-430A-8768-428D47ABCF22}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9023320-1073-430A-8768-428D47ABCF22}">
           <x14:formula1>
             <xm:f>Config!$E$2:$E$4</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Create fill date helper
</commit_message>
<xml_diff>
--- a/Resources/QuickAcq Testplan.xlsx
+++ b/Resources/QuickAcq Testplan.xlsx
@@ -3,8 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Data\Project\selenium\dotnet\LatihanSelenium\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA17C235-4E4D-4DB4-A609-C385E6645D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="9" r:id="rId1"/>
@@ -15,16 +21,16 @@
     <sheet name="RequestForQuotation" sheetId="21" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1"><![CDATA[TestPlan!$A$1:$K$2]]></definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestPlan!$A$1:$K$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr autoRecover="0" crashSave="0" dataExtractLoad="0" repairLoad="0"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -39,267 +45,267 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
-  <si>
-    <t xml:space="preserve">Module Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From Test Case Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screen Capture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screenshot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data For</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attachment Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P@ssw0rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request For Quotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor Quotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save As Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalog / Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Catalog / Non-Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct Purchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Pending Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discard Draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Re Submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods VAT Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services VAT Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pensil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penghapus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License Windows 11 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License Windows 10 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\chris\Downloads\Tips dan Trik untuk Produktivitas Harian- Comserv.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST APPROVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFQ Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFQ Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tender Briefing Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quotation Submission Due Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goods Item Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services Item Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target Appointment Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal Attachment Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor Attachment Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025/01/20 17:04:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit Purchase Request is Fail. Error : OpenQA.Selenium.InvalidElementStateException: invalid element state
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Test Case Id</t>
+  </si>
+  <si>
+    <t>From Test Case Id</t>
+  </si>
+  <si>
+    <t>Date Test</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Screen Capture</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Data For</t>
+  </si>
+  <si>
+    <t>Attachment Path</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Aris</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Purchase Request</t>
+  </si>
+  <si>
+    <t>Request For Quotation</t>
+  </si>
+  <si>
+    <t>Vendor Quotation</t>
+  </si>
+  <si>
+    <t>Vendor Selection</t>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>ROGS</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Save As Draft</t>
+  </si>
+  <si>
+    <t>Submit Draft</t>
+  </si>
+  <si>
+    <t>PR Type</t>
+  </si>
+  <si>
+    <t>Catalog / Contract</t>
+  </si>
+  <si>
+    <t>Non-Catalog / Non-Contract</t>
+  </si>
+  <si>
+    <t>Direct Purchase</t>
+  </si>
+  <si>
+    <t>Search List</t>
+  </si>
+  <si>
+    <t>Search Pending Task</t>
+  </si>
+  <si>
+    <t>Update Draft</t>
+  </si>
+  <si>
+    <t>Discard Draft</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Re Submit</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>PR Subject</t>
+  </si>
+  <si>
+    <t>Required Date</t>
+  </si>
+  <si>
+    <t>Project Code</t>
+  </si>
+  <si>
+    <t>Goods Item Name</t>
+  </si>
+  <si>
+    <t>Goods Item Qty</t>
+  </si>
+  <si>
+    <t>Goods Item Price</t>
+  </si>
+  <si>
+    <t>Services Item Name</t>
+  </si>
+  <si>
+    <t>Services Item Qty</t>
+  </si>
+  <si>
+    <t>Services Item Price</t>
+  </si>
+  <si>
+    <t>Goods VAT Rate</t>
+  </si>
+  <si>
+    <t>Services VAT Rate</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Pensil</t>
+  </si>
+  <si>
+    <t>Buku</t>
+  </si>
+  <si>
+    <t>Penghapus</t>
+  </si>
+  <si>
+    <t>License Windows 11 Pro</t>
+  </si>
+  <si>
+    <t>License Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Document Number</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>C:\Users\chris\Downloads\Tips dan Trik untuk Produktivitas Harian- Comserv.png</t>
+  </si>
+  <si>
+    <t>TEST APPROVE</t>
+  </si>
+  <si>
+    <t>RFQ Subject</t>
+  </si>
+  <si>
+    <t>RFQ Type</t>
+  </si>
+  <si>
+    <t>Tender Briefing Date</t>
+  </si>
+  <si>
+    <t>Quotation Submission Due Date</t>
+  </si>
+  <si>
+    <t>Goods Item Remarks</t>
+  </si>
+  <si>
+    <t>Services Item Remarks</t>
+  </si>
+  <si>
+    <t>Target Appointment Date</t>
+  </si>
+  <si>
+    <t>Internal Attachment Path</t>
+  </si>
+  <si>
+    <t>Vendor Attachment Path</t>
+  </si>
+  <si>
+    <t>2025/01/20 17:04:26</t>
+  </si>
+  <si>
+    <t>Submit Purchase Request is Fail. Error : OpenQA.Selenium.InvalidElementStateException: invalid element state
   (Session info: chrome=131.0.6778.266)
    at OpenQA.Selenium.WebDriver.UnpackAndThrowOnError(Response errorResponse, String commandToExecute)
    at OpenQA.Selenium.WebDriver.ExecuteAsync(String driverCommandToExecute, Dictionary`2 parameters)
@@ -309,20 +315,22 @@
    at LatihanSelenium.Utilities.AutomationHelpers.FillElement(IWebDriver driver, By locator, String param, Int32 sec) in C:\Users\chris\Documents\GitHub\LatihanSelenium\Utilities\AutomationHelpers.cs:line 62</t>
   </si>
   <si>
-    <t xml:space="preserve">Open File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go To Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
+    <t>Open File</t>
+  </si>
+  <si>
+    <t>Go To Data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>21 Jan 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,7 +359,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -425,11 +433,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -697,23 +705,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -753,7 +761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -774,7 +782,7 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -791,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -805,7 +813,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -819,7 +827,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -830,7 +838,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -838,22 +846,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -864,21 +872,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -892,17 +900,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -913,30 +921,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:J2"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -971,33 +979,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>89</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1005,40 +1010,40 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2"/>
+  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="0" count="1">
-    <dataValidation type="list" errorStyle="stop" imeMode="noControl" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1><![CDATA[$A$2:$A$1048576]]></formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>$A$2:$A$1048576</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="I2" location="PurchaseRequest!A2"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I2" location="PurchaseRequest!A2" display="Go To Data" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="4">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DFF4BBE4-322C-43AA-907B-7E8804C69D29}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DFF4BBE4-322C-43AA-907B-7E8804C69D29}">
           <x14:formula1>
             <xm:f>Config!$A$2:$A$1000</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE1FC543-0F99-4865-B769-7910654B9523}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE1FC543-0F99-4865-B769-7910654B9523}">
           <x14:formula1>
             <xm:f>Config!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0065DB-CFB7-4F2F-8F2C-0BC39A6E984A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0065DB-CFB7-4F2F-8F2C-0BC39A6E984A}">
           <x14:formula1>
             <xm:f>User!$B$2:$B$50</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8352D6F0-1E94-47AA-9154-FEE416D3592C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8352D6F0-1E94-47AA-9154-FEE416D3592C}">
           <x14:formula1>
             <xm:f>Config!$B$2:$B$20</xm:f>
           </x14:formula1>
@@ -1051,8 +1056,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1060,17 +1065,17 @@
       <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.44140625" customWidth="1"/>
-    <col min="6" max="6" width="65.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="65.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1093,57 +1098,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F7" s="0"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7"/>
       <c r="G7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="4">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
           <x14:formula1>
             <xm:f>User!$B$2:$B$100</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000004000000}">
           <x14:formula1>
             <xm:f>TestPlan!$A$2:$A$99538</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3E39EE4-6441-4C23-BDD7-10E1293E5F03}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3E39EE4-6441-4C23-BDD7-10E1293E5F03}">
           <x14:formula1>
             <xm:f>Config!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCAF1936-EB14-4904-9946-DB0E2AD5F326}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCAF1936-EB14-4904-9946-DB0E2AD5F326}">
           <x14:formula1>
             <xm:f>Config!$F$2:$F$29</xm:f>
           </x14:formula1>
@@ -1156,28 +1161,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:S9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:I2"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="3" width="8.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="8.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="3" customWidth="1"/>
-    <col min="6" max="9" width="27.44140625" style="3" customWidth="1"/>
-    <col min="10" max="12" width="27.88671875" style="3" customWidth="1"/>
-    <col min="13" max="15" width="27.88671875" customWidth="1"/>
-    <col min="16" max="17" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="3" customWidth="1"/>
+    <col min="6" max="9" width="27.42578125" style="3" customWidth="1"/>
+    <col min="10" max="12" width="27.85546875" style="3" customWidth="1"/>
+    <col min="13" max="15" width="27.85546875" customWidth="1"/>
+    <col min="16" max="17" width="8.5703125" customWidth="1"/>
     <col min="18" max="18" width="32" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1238,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1252,8 +1257,8 @@
       <c r="F2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="11">
-        <v>45677</v>
+      <c r="G2" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>73</v>
@@ -1270,20 +1275,20 @@
       <c r="L2" s="3">
         <v>20000</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="0">
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="O2" s="0">
+      <c r="O2">
         <v>30000</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1302,20 +1307,20 @@
       <c r="L3" s="3">
         <v>2400</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="0">
+      <c r="N3">
         <v>2</v>
       </c>
-      <c r="O3" s="0">
+      <c r="O3">
         <v>3400000</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G9" s="9"/>
     </row>
   </sheetData>
@@ -1346,21 +1351,21 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="3">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
             <xm:f>TestPlan!$A$2:$A$99538</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7071961E-2CD6-4886-8EA4-4BE8922E8D26}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7071961E-2CD6-4886-8EA4-4BE8922E8D26}">
           <x14:formula1>
             <xm:f>Config!$D$2:$D$999</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9023320-1073-430A-8768-428D47ABCF22}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9023320-1073-430A-8768-428D47ABCF22}">
           <x14:formula1>
             <xm:f>Config!$E$2:$E$4</xm:f>
           </x14:formula1>
@@ -1373,21 +1378,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="14" width="31.109375" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="14" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1438,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1448,7 +1452,7 @@
       <c r="K2" s="3"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1462,7 +1466,7 @@
       <c r="K3" s="3"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1479,21 +1483,21 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="3">
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58F7276C-A6B8-40E9-869A-286CC04A775C}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58F7276C-A6B8-40E9-869A-286CC04A775C}">
           <x14:formula1>
             <xm:f>Config!$E$2:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FCBD161-9097-438F-9BDD-88984EF0A9B2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FCBD161-9097-438F-9BDD-88984EF0A9B2}">
           <x14:formula1>
             <xm:f>Config!$D$2:$D$999</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{590AB1A5-E8EA-4FD2-B189-984D3FEAA961}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{590AB1A5-E8EA-4FD2-B189-984D3FEAA961}">
           <x14:formula1>
             <xm:f>TestPlan!$A$2:$A$99538</xm:f>
           </x14:formula1>

</xml_diff>